<commit_message>
Eliminated inaccuracies in the code, in accordance with remarks No. 9
</commit_message>
<xml_diff>
--- a/Test E-dostavka/Constants/Constants.xlsx
+++ b/Test E-dostavka/Constants/Constants.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jurick\Coding\TestProject\Test E-dostavka\Test E-dostavka\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jurick\Coding\TestProject\Test E-dostavka\Test E-dostavka\Constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>123456Aa</t>
   </si>
@@ -32,12 +32,6 @@
     <t>https://e-dostavka.by/</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>D:/Jurick/Coding/TestProject/Test E-dostavka/packages/Selenium.Chrome.WebDriver.85.0.0/driver/</t>
-  </si>
-  <si>
     <t>375296502259</t>
   </si>
   <si>
@@ -59,13 +53,13 @@
     <t>browser</t>
   </si>
   <si>
-    <t>path</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
     <t>Юрий\r\nТеуш</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -389,7 +383,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,49 +395,44 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G2" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Modification of the code in accordance with remarks number 10.
</commit_message>
<xml_diff>
--- a/Test E-dostavka/Constants/Constants.xlsx
+++ b/Test E-dostavka/Constants/Constants.xlsx
@@ -56,10 +56,10 @@
     <t>10</t>
   </si>
   <si>
-    <t>Юрий\r\nТеуш</t>
-  </si>
-  <si>
     <t>firefox</t>
+  </si>
+  <si>
+    <t>Юрий Теуш</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +421,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -430,7 +430,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1"/>
     </row>

</xml_diff>